<commit_message>
modified the bias of post-lasso when n = 120 and m =80
</commit_message>
<xml_diff>
--- a/report_bias_rmse.xlsx
+++ b/report_bias_rmse.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhan Gao\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhan Gao\Documents\Bitbucket\compare_iv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -374,7 +374,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -422,7 +422,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>1.9396</v>
+        <v>0.59630000000000005</v>
       </c>
       <c r="D3">
         <v>0.72550000000000003</v>

</xml_diff>

<commit_message>
updated the bias of post-lasso (120,80)
</commit_message>
<xml_diff>
--- a/report_bias_rmse.xlsx
+++ b/report_bias_rmse.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -404,7 +404,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>7.5800000000000006E-2</v>
+        <v>3.0099999999999998E-2</v>
       </c>
       <c r="D2">
         <v>1.2200000000000001E-2</v>
@@ -442,16 +442,16 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>-1.3599999999999999E-2</v>
+        <v>-1.1900000000000001E-2</v>
       </c>
       <c r="D4">
         <v>-1.7100000000000001E-2</v>
       </c>
       <c r="E4">
-        <v>-6.7999999999999996E-3</v>
+        <v>-6.4000000000000003E-3</v>
       </c>
       <c r="F4">
-        <v>-4.8999999999999998E-3</v>
+        <v>-4.7000000000000002E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -460,16 +460,16 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>8.8999999999999996E-2</v>
+        <v>8.7099999999999997E-2</v>
       </c>
       <c r="D5">
-        <v>0.1208</v>
+        <v>0.1215</v>
       </c>
       <c r="E5">
-        <v>4.7899999999999998E-2</v>
+        <v>4.7699999999999999E-2</v>
       </c>
       <c r="F5">
-        <v>5.6399999999999999E-2</v>
+        <v>5.5899999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New result containing RLIML
</commit_message>
<xml_diff>
--- a/report_bias_rmse.xlsx
+++ b/report_bias_rmse.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>(n = 120, m = 80)</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>RJIVE</t>
+  </si>
+  <si>
+    <t>Rliml</t>
+  </si>
+  <si>
+    <t># outliers</t>
   </si>
 </sst>
 </file>
@@ -371,15 +377,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="6" width="16.59765625" customWidth="1"/>
+    <col min="8" max="8" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
@@ -435,47 +442,140 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>-1.3642861755257901E-2</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>-3.21371858445176E-2</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>-6.1696866669654904E-3</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>-5.2238751227338103E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
-      <c r="B5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>0.100550420901062</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>0.198006246365421</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>4.8154065266145303E-2</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>6.2483419867918097E-2</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>-1.94882109650196E-3</v>
+      </c>
+      <c r="D8">
+        <v>8.4418465313751401E-4</v>
+      </c>
+      <c r="E8">
+        <v>-2.65391534145631E-3</v>
+      </c>
+      <c r="F8">
+        <v>-1.4844115069809799E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>6.9427255325198001E-2</v>
+      </c>
+      <c r="D9">
+        <v>8.9980141564640806E-2</v>
+      </c>
+      <c r="E9">
+        <v>4.3352744458729497E-2</v>
+      </c>
+      <c r="F9">
+        <v>4.7017792876855001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>281</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
replaced fminsearch by fmincon, set upper bound = 4*ones(2,1), lower bound = -6*ones(2,1) algorithm of fmincon: interior-point
</commit_message>
<xml_diff>
--- a/report_bias_rmse.xlsx
+++ b/report_bias_rmse.xlsx
@@ -380,7 +380,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -523,16 +523,16 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>-1.94882109650196E-3</v>
+        <v>-1.9456728912946599E-3</v>
       </c>
       <c r="D8">
-        <v>8.4418465313751401E-4</v>
+        <v>0.252980602052362</v>
       </c>
       <c r="E8">
-        <v>-2.65391534145631E-3</v>
+        <v>-2.6498428005853301E-3</v>
       </c>
       <c r="F8">
-        <v>-1.4844115069809799E-3</v>
+        <v>-1.49115311865267E-3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -541,16 +541,16 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>6.9427255325198001E-2</v>
+        <v>6.9429887590842801E-2</v>
       </c>
       <c r="D9">
-        <v>8.9980141564640806E-2</v>
+        <v>0.95743794735225796</v>
       </c>
       <c r="E9">
-        <v>4.3352744458729497E-2</v>
+        <v>4.3355224262800897E-2</v>
       </c>
       <c r="F9">
-        <v>4.7017792876855001E-2</v>
+        <v>4.7033686592051399E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -562,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>281</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>

</xml_diff>